<commit_message>
added nextion library, Voltage Logger, HMI improved
</commit_message>
<xml_diff>
--- a/Programmierung/CAN_BUS_IDs.xlsx
+++ b/Programmierung/CAN_BUS_IDs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\philipp\git\Diplomarbeit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\philipp\git\Diplomarbeit\Programmierung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A671276F-A626-4FAC-A25B-8979AB92405B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1564F91-EF86-4BBA-86D0-A28CF08E9B50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4128" yWindow="348" windowWidth="9204" windowHeight="9060" xr2:uid="{59229394-A23F-41AD-8842-C58804BC4CA3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59229394-A23F-41AD-8842-C58804BC4CA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -79,6 +79,24 @@
   </si>
   <si>
     <t>CAN_ID_CONTROL_MOTORS_SERVOS</t>
+  </si>
+  <si>
+    <t>CAN_ID_BATTERY_TEMPS_LEFT</t>
+  </si>
+  <si>
+    <t>0xE0</t>
+  </si>
+  <si>
+    <t>CAN_ID_BATTERY_TEMPS_RIGHT</t>
+  </si>
+  <si>
+    <t>0xE1</t>
+  </si>
+  <si>
+    <t>Akku-Temperaturen Links</t>
+  </si>
+  <si>
+    <t>Akku-Temperaturen Rechts</t>
   </si>
 </sst>
 </file>
@@ -439,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32442E77-81F3-40C4-8680-03E66F3A70A4}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,6 +541,34 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
new HMI+ doku weiter
</commit_message>
<xml_diff>
--- a/Programmierung/CAN_BUS_IDs.xlsx
+++ b/Programmierung/CAN_BUS_IDs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\philipp\git\Diplomarbeit\Programmierung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\philipp\git\Diplomarbeit\Programmierung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1564F91-EF86-4BBA-86D0-A28CF08E9B50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4425EAD1-99DA-41E5-97E5-ED2F6FBFA0B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59229394-A23F-41AD-8842-C58804BC4CA3}"/>
+    <workbookView xWindow="2580" yWindow="3370" windowWidth="28800" windowHeight="15460" xr2:uid="{59229394-A23F-41AD-8842-C58804BC4CA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -460,18 +460,18 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" customWidth="1"/>
-    <col min="3" max="3" width="53.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" customWidth="1"/>
+    <col min="3" max="3" width="53.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -485,7 +485,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -499,7 +499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -513,7 +513,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -527,7 +527,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -541,7 +541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -555,7 +555,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
added JetiBox config to protocol
</commit_message>
<xml_diff>
--- a/Programmierung/CAN_BUS_IDs.xlsx
+++ b/Programmierung/CAN_BUS_IDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\philipp\git\Diplomarbeit\Programmierung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4425EAD1-99DA-41E5-97E5-ED2F6FBFA0B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FACD723-ED6A-42D8-B2BD-670A12305AE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="3370" windowWidth="28800" windowHeight="15460" xr2:uid="{59229394-A23F-41AD-8842-C58804BC4CA3}"/>
+    <workbookView xWindow="57480" yWindow="5790" windowWidth="29040" windowHeight="15840" xr2:uid="{59229394-A23F-41AD-8842-C58804BC4CA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -81,22 +81,13 @@
     <t>CAN_ID_CONTROL_MOTORS_SERVOS</t>
   </si>
   <si>
-    <t>CAN_ID_BATTERY_TEMPS_LEFT</t>
-  </si>
-  <si>
     <t>0xE0</t>
   </si>
   <si>
-    <t>CAN_ID_BATTERY_TEMPS_RIGHT</t>
-  </si>
-  <si>
-    <t>0xE1</t>
-  </si>
-  <si>
-    <t>Akku-Temperaturen Links</t>
-  </si>
-  <si>
-    <t>Akku-Temperaturen Rechts</t>
+    <t>CAN_ID_BATTERY_TEMPS</t>
+  </si>
+  <si>
+    <t>Akku-Temperaturen</t>
   </si>
 </sst>
 </file>
@@ -457,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32442E77-81F3-40C4-8680-03E66F3A70A4}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -543,29 +534,15 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7">
         <v>8</v>
       </c>
     </row>

</xml_diff>